<commit_message>
worksheet: add support for IMAGE() future function
</commit_message>
<xml_diff>
--- a/test/perl_output/dynamic_arrays.xlsx
+++ b/test/perl_output/dynamic_arrays.xlsx
@@ -1648,9 +1648,9 @@
       <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" cm="1">
-        <f t="array" ref="D2">_xlfn.XMATCH(C2,A2:A6)</f>
-        <v/>
+      <c r="D2">
+        <f>XMATCH(C2,A2:A6)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4">

</xml_diff>